<commit_message>
Corrected mistakes and updated the .xlsx file
</commit_message>
<xml_diff>
--- a/CountingWords.xlsx
+++ b/CountingWords.xlsx
@@ -428,7 +428,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -461,10 +461,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="3">
-        <v>793</v>
+        <v>861</v>
       </c>
       <c r="D2" s="3">
-        <v>4216</v>
+        <v>6240</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="43.5">
@@ -472,13 +472,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="3">
-        <v>16082</v>
+        <v>6643</v>
       </c>
       <c r="C3" s="3">
-        <v>16082</v>
+        <v>6643</v>
       </c>
       <c r="D3" s="3">
-        <v>16082</v>
+        <v>6643</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="29">
@@ -486,13 +486,13 @@
         <v>6</v>
       </c>
       <c r="B4" s="3">
-        <v>16082</v>
+        <v>6643</v>
       </c>
       <c r="C4" s="3">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D4" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="28.5" customHeight="1">
@@ -500,7 +500,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="3">
-        <v>16082</v>
+        <v>6643</v>
       </c>
       <c r="C5" s="3">
         <v>1</v>
@@ -514,13 +514,13 @@
         <v>8</v>
       </c>
       <c r="B6" s="3">
-        <v>16082</v>
+        <v>6643</v>
       </c>
       <c r="C6" s="3">
-        <v>850</v>
+        <v>38</v>
       </c>
       <c r="D6" s="3">
-        <v>674</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="43.5">
@@ -528,13 +528,13 @@
         <v>9</v>
       </c>
       <c r="B7" s="3">
-        <v>2.911</v>
+        <v>1.4650000000000001</v>
       </c>
       <c r="C7" s="3">
-        <v>0.04</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="D7" s="3">
-        <v>3.5000000000000003E-2</v>
+        <v>1.9E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4">

</xml_diff>